<commit_message>
added fig b8-1 graphic and table b8.2
</commit_message>
<xml_diff>
--- a/input/RESULTS5-2A-BSIMAC-9-9.0.74.xlsx
+++ b/input/RESULTS5-2A-BSIMAC-9-9.0.74.xlsx
@@ -2037,7 +2037,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2045,7 +2045,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2125,19 +2125,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -2332,11 +2332,11 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A146" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D164" activeCellId="0" sqref="D164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
@@ -4702,31 +4702,41 @@
       <c r="B155" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="C155" s="80"/>
+      <c r="C155" s="80" t="n">
+        <v>1670</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="C156" s="83"/>
+      <c r="C156" s="83" t="n">
+        <v>453</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="C157" s="83"/>
+      <c r="C157" s="83" t="n">
+        <v>1061</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C158" s="83"/>
+      <c r="C158" s="83" t="n">
+        <v>1387</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="C159" s="85"/>
+      <c r="C159" s="85" t="n">
+        <v>997</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="38"/>
@@ -4750,25 +4760,33 @@
       <c r="B163" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="C163" s="80"/>
+      <c r="C163" s="80" t="n">
+        <v>820</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="84" t="s">
         <v>146</v>
       </c>
-      <c r="C164" s="83"/>
+      <c r="C164" s="83" t="n">
+        <v>447</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="C165" s="83"/>
+      <c r="C165" s="83" t="n">
+        <v>1037</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="C166" s="85"/>
+      <c r="C166" s="85" t="n">
+        <v>598</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="1"/>
@@ -4791,13 +4809,17 @@
       <c r="B170" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="C170" s="80"/>
+      <c r="C170" s="80" t="n">
+        <v>641</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="C171" s="85"/>
+      <c r="C171" s="85" t="n">
+        <v>438</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="89" t="s">

</xml_diff>

<commit_message>
refactor for section and data update
</commit_message>
<xml_diff>
--- a/input/RESULTS5-2A-BSIMAC-9-9.0.74.xlsx
+++ b/input/RESULTS5-2A-BSIMAC-9-9.0.74.xlsx
@@ -2037,7 +2037,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2045,7 +2045,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2125,19 +2125,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -2332,11 +2332,11 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A146" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D164" activeCellId="0" sqref="D164"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A317" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C330" activeCellId="0" sqref="C330"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
@@ -7730,7 +7730,9 @@
       <c r="B330" s="40" t="n">
         <v>-50</v>
       </c>
-      <c r="C330" s="84"/>
+      <c r="C330" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D330" s="13"/>
       <c r="E330" s="13"/>
     </row>
@@ -7738,7 +7740,9 @@
       <c r="B331" s="40" t="n">
         <v>-49</v>
       </c>
-      <c r="C331" s="84"/>
+      <c r="C331" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D331" s="13"/>
       <c r="E331" s="13"/>
     </row>
@@ -7746,7 +7750,9 @@
       <c r="B332" s="40" t="n">
         <v>-48</v>
       </c>
-      <c r="C332" s="84"/>
+      <c r="C332" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D332" s="13"/>
       <c r="E332" s="13"/>
     </row>
@@ -7754,7 +7760,9 @@
       <c r="B333" s="40" t="n">
         <v>-47</v>
       </c>
-      <c r="C333" s="84"/>
+      <c r="C333" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D333" s="13"/>
       <c r="E333" s="13"/>
     </row>
@@ -7762,7 +7770,9 @@
       <c r="B334" s="40" t="n">
         <v>-46</v>
       </c>
-      <c r="C334" s="84"/>
+      <c r="C334" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D334" s="13"/>
       <c r="E334" s="13"/>
     </row>
@@ -7770,7 +7780,9 @@
       <c r="B335" s="40" t="n">
         <v>-45</v>
       </c>
-      <c r="C335" s="84"/>
+      <c r="C335" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D335" s="13"/>
       <c r="E335" s="13"/>
     </row>
@@ -7778,7 +7790,9 @@
       <c r="B336" s="40" t="n">
         <v>-44</v>
       </c>
-      <c r="C336" s="84"/>
+      <c r="C336" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D336" s="13"/>
       <c r="E336" s="13"/>
     </row>
@@ -7786,7 +7800,9 @@
       <c r="B337" s="40" t="n">
         <v>-43</v>
       </c>
-      <c r="C337" s="84"/>
+      <c r="C337" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D337" s="13"/>
       <c r="E337" s="13"/>
     </row>
@@ -7794,7 +7810,9 @@
       <c r="B338" s="40" t="n">
         <v>-42</v>
       </c>
-      <c r="C338" s="84"/>
+      <c r="C338" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D338" s="13"/>
       <c r="E338" s="13"/>
     </row>
@@ -7802,7 +7820,9 @@
       <c r="B339" s="40" t="n">
         <v>-41</v>
       </c>
-      <c r="C339" s="84"/>
+      <c r="C339" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D339" s="13"/>
       <c r="E339" s="13"/>
     </row>
@@ -7810,7 +7830,9 @@
       <c r="B340" s="40" t="n">
         <v>-40</v>
       </c>
-      <c r="C340" s="84"/>
+      <c r="C340" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D340" s="13"/>
       <c r="E340" s="13"/>
     </row>
@@ -7818,7 +7840,9 @@
       <c r="B341" s="40" t="n">
         <v>-39</v>
       </c>
-      <c r="C341" s="84"/>
+      <c r="C341" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D341" s="13"/>
       <c r="E341" s="13"/>
     </row>
@@ -7826,7 +7850,9 @@
       <c r="B342" s="40" t="n">
         <v>-38</v>
       </c>
-      <c r="C342" s="84"/>
+      <c r="C342" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D342" s="13"/>
       <c r="E342" s="13"/>
     </row>
@@ -7834,7 +7860,9 @@
       <c r="B343" s="40" t="n">
         <v>-37</v>
       </c>
-      <c r="C343" s="84"/>
+      <c r="C343" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D343" s="13"/>
       <c r="E343" s="13"/>
     </row>
@@ -7842,7 +7870,9 @@
       <c r="B344" s="40" t="n">
         <v>-36</v>
       </c>
-      <c r="C344" s="84"/>
+      <c r="C344" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D344" s="13"/>
       <c r="E344" s="13"/>
     </row>
@@ -7850,7 +7880,9 @@
       <c r="B345" s="40" t="n">
         <v>-35</v>
       </c>
-      <c r="C345" s="84"/>
+      <c r="C345" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D345" s="13"/>
       <c r="E345" s="13"/>
     </row>
@@ -7858,7 +7890,9 @@
       <c r="B346" s="40" t="n">
         <v>-34</v>
       </c>
-      <c r="C346" s="84"/>
+      <c r="C346" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D346" s="13"/>
       <c r="E346" s="13"/>
     </row>
@@ -7866,7 +7900,9 @@
       <c r="B347" s="40" t="n">
         <v>-33</v>
       </c>
-      <c r="C347" s="84"/>
+      <c r="C347" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D347" s="13"/>
       <c r="E347" s="13"/>
     </row>
@@ -7874,7 +7910,9 @@
       <c r="B348" s="40" t="n">
         <v>-32</v>
       </c>
-      <c r="C348" s="84"/>
+      <c r="C348" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D348" s="13"/>
       <c r="E348" s="13"/>
     </row>
@@ -7882,7 +7920,9 @@
       <c r="B349" s="40" t="n">
         <v>-31</v>
       </c>
-      <c r="C349" s="84"/>
+      <c r="C349" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D349" s="13"/>
       <c r="E349" s="13"/>
     </row>
@@ -7890,7 +7930,9 @@
       <c r="B350" s="40" t="n">
         <v>-30</v>
       </c>
-      <c r="C350" s="84"/>
+      <c r="C350" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D350" s="13"/>
       <c r="E350" s="13"/>
     </row>
@@ -7898,7 +7940,9 @@
       <c r="B351" s="40" t="n">
         <v>-29</v>
       </c>
-      <c r="C351" s="84"/>
+      <c r="C351" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D351" s="13"/>
       <c r="E351" s="13"/>
     </row>
@@ -7906,7 +7950,9 @@
       <c r="B352" s="40" t="n">
         <v>-28</v>
       </c>
-      <c r="C352" s="84"/>
+      <c r="C352" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D352" s="13"/>
       <c r="E352" s="13"/>
     </row>
@@ -7914,7 +7960,9 @@
       <c r="B353" s="40" t="n">
         <v>-27</v>
       </c>
-      <c r="C353" s="84"/>
+      <c r="C353" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D353" s="13"/>
       <c r="E353" s="13"/>
     </row>
@@ -7922,7 +7970,9 @@
       <c r="B354" s="40" t="n">
         <v>-26</v>
       </c>
-      <c r="C354" s="84"/>
+      <c r="C354" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D354" s="13"/>
       <c r="E354" s="13"/>
     </row>
@@ -7930,7 +7980,9 @@
       <c r="B355" s="40" t="n">
         <v>-25</v>
       </c>
-      <c r="C355" s="84"/>
+      <c r="C355" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D355" s="13"/>
       <c r="E355" s="13"/>
     </row>
@@ -7938,7 +7990,9 @@
       <c r="B356" s="40" t="n">
         <v>-24</v>
       </c>
-      <c r="C356" s="84"/>
+      <c r="C356" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D356" s="13"/>
       <c r="E356" s="13"/>
     </row>
@@ -7946,7 +8000,9 @@
       <c r="B357" s="40" t="n">
         <v>-23</v>
       </c>
-      <c r="C357" s="84"/>
+      <c r="C357" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D357" s="13"/>
       <c r="E357" s="13"/>
     </row>
@@ -7954,7 +8010,9 @@
       <c r="B358" s="40" t="n">
         <v>-22</v>
       </c>
-      <c r="C358" s="84"/>
+      <c r="C358" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D358" s="13"/>
       <c r="E358" s="13"/>
     </row>
@@ -7962,7 +8020,9 @@
       <c r="B359" s="40" t="n">
         <v>-21</v>
       </c>
-      <c r="C359" s="84"/>
+      <c r="C359" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D359" s="13"/>
       <c r="E359" s="13"/>
     </row>
@@ -7970,7 +8030,9 @@
       <c r="B360" s="40" t="n">
         <v>-20</v>
       </c>
-      <c r="C360" s="84"/>
+      <c r="C360" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D360" s="13"/>
       <c r="E360" s="13"/>
     </row>
@@ -7978,7 +8040,9 @@
       <c r="B361" s="40" t="n">
         <v>-19</v>
       </c>
-      <c r="C361" s="84"/>
+      <c r="C361" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D361" s="13"/>
       <c r="E361" s="13"/>
     </row>
@@ -7986,7 +8050,9 @@
       <c r="B362" s="40" t="n">
         <v>-18</v>
       </c>
-      <c r="C362" s="84"/>
+      <c r="C362" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D362" s="13"/>
       <c r="E362" s="13"/>
     </row>
@@ -7994,7 +8060,9 @@
       <c r="B363" s="40" t="n">
         <v>-17</v>
       </c>
-      <c r="C363" s="84"/>
+      <c r="C363" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D363" s="13"/>
       <c r="E363" s="13"/>
     </row>
@@ -8002,7 +8070,9 @@
       <c r="B364" s="40" t="n">
         <v>-16</v>
       </c>
-      <c r="C364" s="84"/>
+      <c r="C364" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D364" s="13"/>
       <c r="E364" s="13"/>
     </row>
@@ -8010,7 +8080,9 @@
       <c r="B365" s="40" t="n">
         <v>-15</v>
       </c>
-      <c r="C365" s="84"/>
+      <c r="C365" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D365" s="13"/>
       <c r="E365" s="13"/>
     </row>
@@ -8018,7 +8090,9 @@
       <c r="B366" s="40" t="n">
         <v>-14</v>
       </c>
-      <c r="C366" s="84"/>
+      <c r="C366" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D366" s="13"/>
       <c r="E366" s="13"/>
     </row>
@@ -8026,7 +8100,9 @@
       <c r="B367" s="40" t="n">
         <v>-13</v>
       </c>
-      <c r="C367" s="84"/>
+      <c r="C367" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D367" s="13"/>
       <c r="E367" s="13"/>
     </row>
@@ -8034,7 +8110,9 @@
       <c r="B368" s="40" t="n">
         <v>-12</v>
       </c>
-      <c r="C368" s="84"/>
+      <c r="C368" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D368" s="13"/>
       <c r="E368" s="13"/>
     </row>
@@ -8042,7 +8120,9 @@
       <c r="B369" s="40" t="n">
         <v>-11</v>
       </c>
-      <c r="C369" s="84"/>
+      <c r="C369" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D369" s="13"/>
       <c r="E369" s="13"/>
     </row>
@@ -8050,7 +8130,9 @@
       <c r="B370" s="40" t="n">
         <v>-10</v>
       </c>
-      <c r="C370" s="84"/>
+      <c r="C370" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D370" s="13"/>
       <c r="E370" s="13"/>
     </row>
@@ -8058,7 +8140,9 @@
       <c r="B371" s="40" t="n">
         <v>-9</v>
       </c>
-      <c r="C371" s="84"/>
+      <c r="C371" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D371" s="13"/>
       <c r="E371" s="13"/>
     </row>
@@ -8066,7 +8150,9 @@
       <c r="B372" s="40" t="n">
         <v>-8</v>
       </c>
-      <c r="C372" s="84"/>
+      <c r="C372" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D372" s="13"/>
       <c r="E372" s="13"/>
     </row>
@@ -8074,7 +8160,9 @@
       <c r="B373" s="40" t="n">
         <v>-7</v>
       </c>
-      <c r="C373" s="84"/>
+      <c r="C373" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D373" s="13"/>
       <c r="E373" s="13"/>
     </row>
@@ -8082,7 +8170,9 @@
       <c r="B374" s="40" t="n">
         <v>-6</v>
       </c>
-      <c r="C374" s="84"/>
+      <c r="C374" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D374" s="13"/>
       <c r="E374" s="13"/>
     </row>
@@ -8090,7 +8180,9 @@
       <c r="B375" s="40" t="n">
         <v>-5</v>
       </c>
-      <c r="C375" s="84"/>
+      <c r="C375" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D375" s="13"/>
       <c r="E375" s="13"/>
     </row>
@@ -8098,7 +8190,9 @@
       <c r="B376" s="40" t="n">
         <v>-4</v>
       </c>
-      <c r="C376" s="84"/>
+      <c r="C376" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D376" s="13"/>
       <c r="E376" s="13"/>
     </row>
@@ -8106,7 +8200,9 @@
       <c r="B377" s="40" t="n">
         <v>-3</v>
       </c>
-      <c r="C377" s="84"/>
+      <c r="C377" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D377" s="13"/>
       <c r="E377" s="13"/>
     </row>
@@ -8114,7 +8210,9 @@
       <c r="B378" s="40" t="n">
         <v>-2</v>
       </c>
-      <c r="C378" s="84"/>
+      <c r="C378" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D378" s="13"/>
       <c r="E378" s="13"/>
     </row>
@@ -8122,7 +8220,9 @@
       <c r="B379" s="40" t="n">
         <v>-1</v>
       </c>
-      <c r="C379" s="84"/>
+      <c r="C379" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D379" s="13"/>
       <c r="E379" s="13"/>
     </row>
@@ -8130,7 +8230,9 @@
       <c r="B380" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="C380" s="84"/>
+      <c r="C380" s="84" t="n">
+        <v>3</v>
+      </c>
       <c r="D380" s="13"/>
       <c r="E380" s="13"/>
     </row>
@@ -8138,7 +8240,9 @@
       <c r="B381" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="C381" s="84"/>
+      <c r="C381" s="84" t="n">
+        <v>13</v>
+      </c>
       <c r="D381" s="13"/>
       <c r="E381" s="13"/>
     </row>
@@ -8146,7 +8250,9 @@
       <c r="B382" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="C382" s="84"/>
+      <c r="C382" s="84" t="n">
+        <v>32</v>
+      </c>
       <c r="D382" s="13"/>
       <c r="E382" s="13"/>
     </row>
@@ -8154,7 +8260,9 @@
       <c r="B383" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="C383" s="84"/>
+      <c r="C383" s="84" t="n">
+        <v>41</v>
+      </c>
       <c r="D383" s="13"/>
       <c r="E383" s="13"/>
     </row>
@@ -8162,7 +8270,9 @@
       <c r="B384" s="40" t="n">
         <v>4</v>
       </c>
-      <c r="C384" s="84"/>
+      <c r="C384" s="84" t="n">
+        <v>57</v>
+      </c>
       <c r="D384" s="13"/>
       <c r="E384" s="13"/>
     </row>
@@ -8170,7 +8280,9 @@
       <c r="B385" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="C385" s="84"/>
+      <c r="C385" s="84" t="n">
+        <v>63</v>
+      </c>
       <c r="D385" s="13"/>
       <c r="E385" s="13"/>
     </row>
@@ -8178,7 +8290,9 @@
       <c r="B386" s="40" t="n">
         <v>6</v>
       </c>
-      <c r="C386" s="84"/>
+      <c r="C386" s="84" t="n">
+        <v>67</v>
+      </c>
       <c r="D386" s="13"/>
       <c r="E386" s="13"/>
     </row>
@@ -8186,7 +8300,9 @@
       <c r="B387" s="40" t="n">
         <v>7</v>
       </c>
-      <c r="C387" s="84"/>
+      <c r="C387" s="84" t="n">
+        <v>87</v>
+      </c>
       <c r="D387" s="13"/>
       <c r="E387" s="13"/>
     </row>
@@ -8194,7 +8310,9 @@
       <c r="B388" s="40" t="n">
         <v>8</v>
       </c>
-      <c r="C388" s="84"/>
+      <c r="C388" s="84" t="n">
+        <v>97</v>
+      </c>
       <c r="D388" s="13"/>
       <c r="E388" s="13"/>
     </row>
@@ -8202,7 +8320,9 @@
       <c r="B389" s="40" t="n">
         <v>9</v>
       </c>
-      <c r="C389" s="84"/>
+      <c r="C389" s="84" t="n">
+        <v>104</v>
+      </c>
       <c r="D389" s="13"/>
       <c r="E389" s="13"/>
     </row>
@@ -8210,7 +8330,9 @@
       <c r="B390" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="C390" s="84"/>
+      <c r="C390" s="84" t="n">
+        <v>155</v>
+      </c>
       <c r="D390" s="13"/>
       <c r="E390" s="13"/>
     </row>
@@ -8218,7 +8340,9 @@
       <c r="B391" s="40" t="n">
         <v>11</v>
       </c>
-      <c r="C391" s="84"/>
+      <c r="C391" s="84" t="n">
+        <v>151</v>
+      </c>
       <c r="D391" s="13"/>
       <c r="E391" s="13"/>
     </row>
@@ -8226,7 +8350,9 @@
       <c r="B392" s="40" t="n">
         <v>12</v>
       </c>
-      <c r="C392" s="84"/>
+      <c r="C392" s="84" t="n">
+        <v>142</v>
+      </c>
       <c r="D392" s="13"/>
       <c r="E392" s="13"/>
     </row>
@@ -8234,7 +8360,9 @@
       <c r="B393" s="40" t="n">
         <v>13</v>
       </c>
-      <c r="C393" s="84"/>
+      <c r="C393" s="84" t="n">
+        <v>156</v>
+      </c>
       <c r="D393" s="13"/>
       <c r="E393" s="13"/>
     </row>
@@ -8242,7 +8370,9 @@
       <c r="B394" s="40" t="n">
         <v>14</v>
       </c>
-      <c r="C394" s="84"/>
+      <c r="C394" s="84" t="n">
+        <v>170</v>
+      </c>
       <c r="D394" s="13"/>
       <c r="E394" s="13"/>
     </row>
@@ -8250,7 +8380,9 @@
       <c r="B395" s="40" t="n">
         <v>15</v>
       </c>
-      <c r="C395" s="84"/>
+      <c r="C395" s="84" t="n">
+        <v>166</v>
+      </c>
       <c r="D395" s="13"/>
       <c r="E395" s="13"/>
     </row>
@@ -8258,7 +8390,9 @@
       <c r="B396" s="40" t="n">
         <v>16</v>
       </c>
-      <c r="C396" s="84"/>
+      <c r="C396" s="84" t="n">
+        <v>211</v>
+      </c>
       <c r="D396" s="13"/>
       <c r="E396" s="13"/>
     </row>
@@ -8266,7 +8400,9 @@
       <c r="B397" s="40" t="n">
         <v>17</v>
       </c>
-      <c r="C397" s="84"/>
+      <c r="C397" s="84" t="n">
+        <v>199</v>
+      </c>
       <c r="D397" s="13"/>
       <c r="E397" s="13"/>
     </row>
@@ -8274,7 +8410,9 @@
       <c r="B398" s="40" t="n">
         <v>18</v>
       </c>
-      <c r="C398" s="84"/>
+      <c r="C398" s="84" t="n">
+        <v>211</v>
+      </c>
       <c r="D398" s="13"/>
       <c r="E398" s="13"/>
     </row>
@@ -8282,7 +8420,9 @@
       <c r="B399" s="40" t="n">
         <v>19</v>
       </c>
-      <c r="C399" s="84"/>
+      <c r="C399" s="84" t="n">
+        <v>257</v>
+      </c>
       <c r="D399" s="13"/>
       <c r="E399" s="13"/>
     </row>
@@ -8290,7 +8430,9 @@
       <c r="B400" s="40" t="n">
         <v>20</v>
       </c>
-      <c r="C400" s="84"/>
+      <c r="C400" s="84" t="n">
+        <v>318</v>
+      </c>
       <c r="D400" s="13"/>
       <c r="E400" s="13"/>
     </row>
@@ -8298,7 +8440,9 @@
       <c r="B401" s="40" t="n">
         <v>21</v>
       </c>
-      <c r="C401" s="84"/>
+      <c r="C401" s="84" t="n">
+        <v>263</v>
+      </c>
       <c r="D401" s="13"/>
       <c r="E401" s="13"/>
     </row>
@@ -8306,7 +8450,9 @@
       <c r="B402" s="40" t="n">
         <v>22</v>
       </c>
-      <c r="C402" s="84"/>
+      <c r="C402" s="84" t="n">
+        <v>269</v>
+      </c>
       <c r="D402" s="13"/>
       <c r="E402" s="13"/>
     </row>
@@ -8314,7 +8460,9 @@
       <c r="B403" s="40" t="n">
         <v>23</v>
       </c>
-      <c r="C403" s="84"/>
+      <c r="C403" s="84" t="n">
+        <v>273</v>
+      </c>
       <c r="D403" s="13"/>
       <c r="E403" s="13"/>
     </row>
@@ -8322,7 +8470,9 @@
       <c r="B404" s="40" t="n">
         <v>24</v>
       </c>
-      <c r="C404" s="84"/>
+      <c r="C404" s="84" t="n">
+        <v>260</v>
+      </c>
       <c r="D404" s="13"/>
       <c r="E404" s="13"/>
     </row>
@@ -8330,7 +8480,9 @@
       <c r="B405" s="40" t="n">
         <v>25</v>
       </c>
-      <c r="C405" s="84"/>
+      <c r="C405" s="84" t="n">
+        <v>308</v>
+      </c>
       <c r="D405" s="13"/>
       <c r="E405" s="13"/>
     </row>
@@ -8338,7 +8490,9 @@
       <c r="B406" s="40" t="n">
         <v>26</v>
       </c>
-      <c r="C406" s="84"/>
+      <c r="C406" s="84" t="n">
+        <v>339</v>
+      </c>
       <c r="D406" s="13"/>
       <c r="E406" s="13"/>
     </row>
@@ -8346,7 +8500,9 @@
       <c r="B407" s="40" t="n">
         <v>27</v>
       </c>
-      <c r="C407" s="84"/>
+      <c r="C407" s="84" t="n">
+        <v>330</v>
+      </c>
       <c r="D407" s="13"/>
       <c r="E407" s="13"/>
     </row>
@@ -8354,7 +8510,9 @@
       <c r="B408" s="40" t="n">
         <v>28</v>
       </c>
-      <c r="C408" s="84"/>
+      <c r="C408" s="84" t="n">
+        <v>341</v>
+      </c>
       <c r="D408" s="13"/>
       <c r="E408" s="13"/>
     </row>
@@ -8362,7 +8520,9 @@
       <c r="B409" s="40" t="n">
         <v>29</v>
       </c>
-      <c r="C409" s="84"/>
+      <c r="C409" s="84" t="n">
+        <v>409</v>
+      </c>
       <c r="D409" s="13"/>
       <c r="E409" s="13"/>
     </row>
@@ -8370,7 +8530,9 @@
       <c r="B410" s="40" t="n">
         <v>30</v>
       </c>
-      <c r="C410" s="84"/>
+      <c r="C410" s="84" t="n">
+        <v>382</v>
+      </c>
       <c r="D410" s="13"/>
       <c r="E410" s="13"/>
     </row>
@@ -8378,7 +8540,9 @@
       <c r="B411" s="40" t="n">
         <v>31</v>
       </c>
-      <c r="C411" s="84"/>
+      <c r="C411" s="84" t="n">
+        <v>426</v>
+      </c>
       <c r="D411" s="13"/>
       <c r="E411" s="13"/>
     </row>
@@ -8386,7 +8550,9 @@
       <c r="B412" s="40" t="n">
         <v>32</v>
       </c>
-      <c r="C412" s="84"/>
+      <c r="C412" s="84" t="n">
+        <v>433</v>
+      </c>
       <c r="D412" s="13"/>
       <c r="E412" s="13"/>
     </row>
@@ -8394,7 +8560,9 @@
       <c r="B413" s="40" t="n">
         <v>33</v>
       </c>
-      <c r="C413" s="84"/>
+      <c r="C413" s="84" t="n">
+        <v>391</v>
+      </c>
       <c r="D413" s="13"/>
       <c r="E413" s="13"/>
     </row>
@@ -8402,7 +8570,9 @@
       <c r="B414" s="40" t="n">
         <v>34</v>
       </c>
-      <c r="C414" s="84"/>
+      <c r="C414" s="84" t="n">
+        <v>332</v>
+      </c>
       <c r="D414" s="13"/>
       <c r="E414" s="13"/>
     </row>
@@ -8410,7 +8580,9 @@
       <c r="B415" s="40" t="n">
         <v>35</v>
       </c>
-      <c r="C415" s="84"/>
+      <c r="C415" s="84" t="n">
+        <v>291</v>
+      </c>
       <c r="D415" s="13"/>
       <c r="E415" s="13"/>
     </row>
@@ -8418,7 +8590,9 @@
       <c r="B416" s="40" t="n">
         <v>36</v>
       </c>
-      <c r="C416" s="84"/>
+      <c r="C416" s="84" t="n">
+        <v>244</v>
+      </c>
       <c r="D416" s="13"/>
       <c r="E416" s="13"/>
     </row>
@@ -8426,7 +8600,9 @@
       <c r="B417" s="40" t="n">
         <v>37</v>
       </c>
-      <c r="C417" s="84"/>
+      <c r="C417" s="84" t="n">
+        <v>184</v>
+      </c>
       <c r="D417" s="13"/>
       <c r="E417" s="13"/>
     </row>
@@ -8434,7 +8610,9 @@
       <c r="B418" s="40" t="n">
         <v>38</v>
       </c>
-      <c r="C418" s="84"/>
+      <c r="C418" s="84" t="n">
+        <v>167</v>
+      </c>
       <c r="D418" s="13"/>
       <c r="E418" s="13"/>
     </row>
@@ -8442,7 +8620,9 @@
       <c r="B419" s="40" t="n">
         <v>39</v>
       </c>
-      <c r="C419" s="84"/>
+      <c r="C419" s="84" t="n">
+        <v>145</v>
+      </c>
       <c r="D419" s="13"/>
       <c r="E419" s="13"/>
     </row>
@@ -8450,7 +8630,9 @@
       <c r="B420" s="40" t="n">
         <v>40</v>
       </c>
-      <c r="C420" s="84"/>
+      <c r="C420" s="84" t="n">
+        <v>102</v>
+      </c>
       <c r="D420" s="13"/>
       <c r="E420" s="13"/>
     </row>
@@ -8458,7 +8640,9 @@
       <c r="B421" s="40" t="n">
         <v>41</v>
       </c>
-      <c r="C421" s="84"/>
+      <c r="C421" s="84" t="n">
+        <v>76</v>
+      </c>
       <c r="D421" s="13"/>
       <c r="E421" s="13"/>
     </row>
@@ -8466,7 +8650,9 @@
       <c r="B422" s="40" t="n">
         <v>42</v>
       </c>
-      <c r="C422" s="84"/>
+      <c r="C422" s="84" t="n">
+        <v>41</v>
+      </c>
       <c r="D422" s="13"/>
       <c r="E422" s="13"/>
     </row>
@@ -8474,7 +8660,9 @@
       <c r="B423" s="40" t="n">
         <v>43</v>
       </c>
-      <c r="C423" s="84"/>
+      <c r="C423" s="84" t="n">
+        <v>27</v>
+      </c>
       <c r="D423" s="13"/>
       <c r="E423" s="13"/>
     </row>
@@ -8482,7 +8670,9 @@
       <c r="B424" s="40" t="n">
         <v>44</v>
       </c>
-      <c r="C424" s="84"/>
+      <c r="C424" s="84" t="n">
+        <v>22</v>
+      </c>
       <c r="D424" s="13"/>
       <c r="E424" s="13"/>
     </row>
@@ -8490,7 +8680,9 @@
       <c r="B425" s="40" t="n">
         <v>45</v>
       </c>
-      <c r="C425" s="84"/>
+      <c r="C425" s="84" t="n">
+        <v>5</v>
+      </c>
       <c r="D425" s="13"/>
       <c r="E425" s="13"/>
     </row>
@@ -8498,7 +8690,9 @@
       <c r="B426" s="40" t="n">
         <v>46</v>
       </c>
-      <c r="C426" s="84"/>
+      <c r="C426" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D426" s="13"/>
       <c r="E426" s="13"/>
     </row>
@@ -8506,7 +8700,9 @@
       <c r="B427" s="40" t="n">
         <v>47</v>
       </c>
-      <c r="C427" s="84"/>
+      <c r="C427" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D427" s="13"/>
       <c r="E427" s="13"/>
     </row>
@@ -8514,7 +8710,9 @@
       <c r="B428" s="40" t="n">
         <v>48</v>
       </c>
-      <c r="C428" s="84"/>
+      <c r="C428" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D428" s="13"/>
       <c r="E428" s="13"/>
     </row>
@@ -8522,7 +8720,9 @@
       <c r="B429" s="40" t="n">
         <v>49</v>
       </c>
-      <c r="C429" s="84"/>
+      <c r="C429" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D429" s="13"/>
       <c r="E429" s="13"/>
     </row>
@@ -8530,7 +8730,9 @@
       <c r="B430" s="40" t="n">
         <v>50</v>
       </c>
-      <c r="C430" s="84"/>
+      <c r="C430" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D430" s="13"/>
       <c r="E430" s="13"/>
     </row>
@@ -8538,7 +8740,9 @@
       <c r="B431" s="40" t="n">
         <v>51</v>
       </c>
-      <c r="C431" s="84"/>
+      <c r="C431" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D431" s="13"/>
       <c r="E431" s="13"/>
     </row>
@@ -8546,7 +8750,9 @@
       <c r="B432" s="40" t="n">
         <v>52</v>
       </c>
-      <c r="C432" s="84"/>
+      <c r="C432" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D432" s="13"/>
       <c r="E432" s="13"/>
     </row>
@@ -8554,7 +8760,9 @@
       <c r="B433" s="40" t="n">
         <v>53</v>
       </c>
-      <c r="C433" s="84"/>
+      <c r="C433" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D433" s="13"/>
       <c r="E433" s="13"/>
     </row>
@@ -8562,7 +8770,9 @@
       <c r="B434" s="40" t="n">
         <v>54</v>
       </c>
-      <c r="C434" s="84"/>
+      <c r="C434" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D434" s="13"/>
       <c r="E434" s="13"/>
     </row>
@@ -8570,7 +8780,9 @@
       <c r="B435" s="40" t="n">
         <v>55</v>
       </c>
-      <c r="C435" s="84"/>
+      <c r="C435" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D435" s="13"/>
       <c r="E435" s="13"/>
     </row>
@@ -8578,7 +8790,9 @@
       <c r="B436" s="40" t="n">
         <v>56</v>
       </c>
-      <c r="C436" s="84"/>
+      <c r="C436" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D436" s="13"/>
       <c r="E436" s="13"/>
     </row>
@@ -8586,7 +8800,9 @@
       <c r="B437" s="40" t="n">
         <v>57</v>
       </c>
-      <c r="C437" s="84"/>
+      <c r="C437" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D437" s="13"/>
       <c r="E437" s="13"/>
     </row>
@@ -8594,7 +8810,9 @@
       <c r="B438" s="40" t="n">
         <v>58</v>
       </c>
-      <c r="C438" s="84"/>
+      <c r="C438" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D438" s="13"/>
       <c r="E438" s="13"/>
     </row>
@@ -8602,7 +8820,9 @@
       <c r="B439" s="40" t="n">
         <v>59</v>
       </c>
-      <c r="C439" s="84"/>
+      <c r="C439" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D439" s="13"/>
       <c r="E439" s="13"/>
     </row>
@@ -8610,7 +8830,9 @@
       <c r="B440" s="40" t="n">
         <v>60</v>
       </c>
-      <c r="C440" s="84"/>
+      <c r="C440" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D440" s="13"/>
       <c r="E440" s="13"/>
     </row>
@@ -8618,7 +8840,9 @@
       <c r="B441" s="40" t="n">
         <v>61</v>
       </c>
-      <c r="C441" s="84"/>
+      <c r="C441" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D441" s="13"/>
       <c r="E441" s="13"/>
     </row>
@@ -8626,7 +8850,9 @@
       <c r="B442" s="40" t="n">
         <v>62</v>
       </c>
-      <c r="C442" s="84"/>
+      <c r="C442" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D442" s="13"/>
       <c r="E442" s="13"/>
     </row>
@@ -8634,7 +8860,9 @@
       <c r="B443" s="40" t="n">
         <v>63</v>
       </c>
-      <c r="C443" s="84"/>
+      <c r="C443" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D443" s="13"/>
       <c r="E443" s="13"/>
     </row>
@@ -8642,7 +8870,9 @@
       <c r="B444" s="40" t="n">
         <v>64</v>
       </c>
-      <c r="C444" s="84"/>
+      <c r="C444" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D444" s="13"/>
       <c r="E444" s="13"/>
     </row>
@@ -8650,7 +8880,9 @@
       <c r="B445" s="40" t="n">
         <v>65</v>
       </c>
-      <c r="C445" s="84"/>
+      <c r="C445" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D445" s="13"/>
       <c r="E445" s="13"/>
     </row>
@@ -8658,7 +8890,9 @@
       <c r="B446" s="40" t="n">
         <v>66</v>
       </c>
-      <c r="C446" s="84"/>
+      <c r="C446" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D446" s="13"/>
       <c r="E446" s="13"/>
     </row>
@@ -8666,7 +8900,9 @@
       <c r="B447" s="40" t="n">
         <v>67</v>
       </c>
-      <c r="C447" s="84"/>
+      <c r="C447" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D447" s="13"/>
       <c r="E447" s="13"/>
     </row>
@@ -8674,7 +8910,9 @@
       <c r="B448" s="40" t="n">
         <v>68</v>
       </c>
-      <c r="C448" s="84"/>
+      <c r="C448" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D448" s="13"/>
       <c r="E448" s="13"/>
     </row>
@@ -8682,7 +8920,9 @@
       <c r="B449" s="40" t="n">
         <v>69</v>
       </c>
-      <c r="C449" s="84"/>
+      <c r="C449" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D449" s="13"/>
       <c r="E449" s="13"/>
     </row>
@@ -8690,7 +8930,9 @@
       <c r="B450" s="40" t="n">
         <v>70</v>
       </c>
-      <c r="C450" s="84"/>
+      <c r="C450" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D450" s="13"/>
       <c r="E450" s="13"/>
     </row>
@@ -8698,7 +8940,9 @@
       <c r="B451" s="40" t="n">
         <v>71</v>
       </c>
-      <c r="C451" s="84"/>
+      <c r="C451" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D451" s="13"/>
       <c r="E451" s="13"/>
     </row>
@@ -8706,7 +8950,9 @@
       <c r="B452" s="40" t="n">
         <v>72</v>
       </c>
-      <c r="C452" s="84"/>
+      <c r="C452" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D452" s="13"/>
       <c r="E452" s="13"/>
     </row>
@@ -8714,7 +8960,9 @@
       <c r="B453" s="40" t="n">
         <v>73</v>
       </c>
-      <c r="C453" s="84"/>
+      <c r="C453" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D453" s="13"/>
       <c r="E453" s="13"/>
     </row>
@@ -8722,7 +8970,9 @@
       <c r="B454" s="40" t="n">
         <v>74</v>
       </c>
-      <c r="C454" s="84"/>
+      <c r="C454" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D454" s="13"/>
       <c r="E454" s="13"/>
     </row>
@@ -8730,7 +8980,9 @@
       <c r="B455" s="40" t="n">
         <v>75</v>
       </c>
-      <c r="C455" s="84"/>
+      <c r="C455" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D455" s="13"/>
       <c r="E455" s="13"/>
     </row>
@@ -8738,7 +8990,9 @@
       <c r="B456" s="40" t="n">
         <v>76</v>
       </c>
-      <c r="C456" s="84"/>
+      <c r="C456" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D456" s="13"/>
       <c r="E456" s="13"/>
     </row>
@@ -8746,7 +9000,9 @@
       <c r="B457" s="40" t="n">
         <v>77</v>
       </c>
-      <c r="C457" s="84"/>
+      <c r="C457" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D457" s="13"/>
       <c r="E457" s="13"/>
     </row>
@@ -8754,7 +9010,9 @@
       <c r="B458" s="40" t="n">
         <v>78</v>
       </c>
-      <c r="C458" s="84"/>
+      <c r="C458" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D458" s="13"/>
       <c r="E458" s="13"/>
     </row>
@@ -8762,7 +9020,9 @@
       <c r="B459" s="40" t="n">
         <v>79</v>
       </c>
-      <c r="C459" s="84"/>
+      <c r="C459" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D459" s="13"/>
       <c r="E459" s="13"/>
     </row>
@@ -8770,7 +9030,9 @@
       <c r="B460" s="40" t="n">
         <v>80</v>
       </c>
-      <c r="C460" s="84"/>
+      <c r="C460" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D460" s="13"/>
       <c r="E460" s="13"/>
     </row>
@@ -8778,7 +9040,9 @@
       <c r="B461" s="40" t="n">
         <v>81</v>
       </c>
-      <c r="C461" s="84"/>
+      <c r="C461" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D461" s="13"/>
       <c r="E461" s="13"/>
     </row>
@@ -8786,7 +9050,9 @@
       <c r="B462" s="40" t="n">
         <v>82</v>
       </c>
-      <c r="C462" s="84"/>
+      <c r="C462" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D462" s="13"/>
       <c r="E462" s="13"/>
     </row>
@@ -8794,7 +9060,9 @@
       <c r="B463" s="40" t="n">
         <v>83</v>
       </c>
-      <c r="C463" s="84"/>
+      <c r="C463" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D463" s="13"/>
       <c r="E463" s="13"/>
     </row>
@@ -8802,7 +9070,9 @@
       <c r="B464" s="40" t="n">
         <v>84</v>
       </c>
-      <c r="C464" s="84"/>
+      <c r="C464" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D464" s="13"/>
       <c r="E464" s="13"/>
     </row>
@@ -8810,7 +9080,9 @@
       <c r="B465" s="40" t="n">
         <v>85</v>
       </c>
-      <c r="C465" s="84"/>
+      <c r="C465" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D465" s="13"/>
       <c r="E465" s="13"/>
     </row>
@@ -8818,7 +9090,9 @@
       <c r="B466" s="40" t="n">
         <v>86</v>
       </c>
-      <c r="C466" s="84"/>
+      <c r="C466" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D466" s="13"/>
       <c r="E466" s="13"/>
     </row>
@@ -8826,7 +9100,9 @@
       <c r="B467" s="40" t="n">
         <v>87</v>
       </c>
-      <c r="C467" s="84"/>
+      <c r="C467" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D467" s="13"/>
       <c r="E467" s="13"/>
     </row>
@@ -8834,7 +9110,9 @@
       <c r="B468" s="40" t="n">
         <v>88</v>
       </c>
-      <c r="C468" s="84"/>
+      <c r="C468" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D468" s="13"/>
       <c r="E468" s="13"/>
     </row>
@@ -8842,7 +9120,9 @@
       <c r="B469" s="40" t="n">
         <v>89</v>
       </c>
-      <c r="C469" s="84"/>
+      <c r="C469" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D469" s="13"/>
       <c r="E469" s="13"/>
     </row>
@@ -8850,7 +9130,9 @@
       <c r="B470" s="40" t="n">
         <v>90</v>
       </c>
-      <c r="C470" s="84"/>
+      <c r="C470" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D470" s="13"/>
       <c r="E470" s="13"/>
     </row>
@@ -8858,7 +9140,9 @@
       <c r="B471" s="40" t="n">
         <v>91</v>
       </c>
-      <c r="C471" s="84"/>
+      <c r="C471" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D471" s="13"/>
       <c r="E471" s="13"/>
     </row>
@@ -8866,7 +9150,9 @@
       <c r="B472" s="40" t="n">
         <v>92</v>
       </c>
-      <c r="C472" s="84"/>
+      <c r="C472" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D472" s="13"/>
       <c r="E472" s="13"/>
     </row>
@@ -8874,7 +9160,9 @@
       <c r="B473" s="40" t="n">
         <v>93</v>
       </c>
-      <c r="C473" s="84"/>
+      <c r="C473" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D473" s="13"/>
       <c r="E473" s="13"/>
     </row>
@@ -8882,7 +9170,9 @@
       <c r="B474" s="40" t="n">
         <v>94</v>
       </c>
-      <c r="C474" s="84"/>
+      <c r="C474" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D474" s="13"/>
       <c r="E474" s="13"/>
     </row>
@@ -8890,7 +9180,9 @@
       <c r="B475" s="40" t="n">
         <v>95</v>
       </c>
-      <c r="C475" s="84"/>
+      <c r="C475" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D475" s="13"/>
       <c r="E475" s="13"/>
     </row>
@@ -8898,7 +9190,9 @@
       <c r="B476" s="40" t="n">
         <v>96</v>
       </c>
-      <c r="C476" s="84"/>
+      <c r="C476" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D476" s="13"/>
       <c r="E476" s="13"/>
     </row>
@@ -8906,7 +9200,9 @@
       <c r="B477" s="40" t="n">
         <v>97</v>
       </c>
-      <c r="C477" s="84"/>
+      <c r="C477" s="84" t="n">
+        <v>0</v>
+      </c>
       <c r="D477" s="13"/>
       <c r="E477" s="13" t="s">
         <v>203</v>
@@ -8916,11 +9212,13 @@
       <c r="B478" s="47" t="n">
         <v>98</v>
       </c>
-      <c r="C478" s="100"/>
+      <c r="C478" s="100" t="n">
+        <v>0</v>
+      </c>
       <c r="D478" s="13"/>
       <c r="E478" s="13" t="n">
         <f aca="false">SUM(C330:C478)</f>
-        <v>0</v>
+        <v>8760</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>